<commit_message>
add doc_firmado and email config
</commit_message>
<xml_diff>
--- a/public/formatos/informe_ideas.xlsx
+++ b/public/formatos/informe_ideas.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Usuario\Documents\WebProjects\LaravelProjects\sistemas-app\public\formatos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{88274800-0CB8-457B-B230-5D0C435417BD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{08FCA94A-1A30-4553-B244-ACF6D90B4D15}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{1738465B-6626-4A91-BE06-82A6A58D01DC}"/>
   </bookViews>
@@ -78,9 +78,6 @@
     </r>
   </si>
   <si>
-    <t>Titúlo de la idea</t>
-  </si>
-  <si>
     <t>Objetivo</t>
   </si>
   <si>
@@ -91,6 +88,9 @@
   </si>
   <si>
     <t>Periodo</t>
+  </si>
+  <si>
+    <t>Título de la idea</t>
   </si>
 </sst>
 </file>
@@ -638,7 +638,7 @@
   <dimension ref="A1:I2"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -672,10 +672,10 @@
         <v>0</v>
       </c>
       <c r="B2" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="C2" s="5" t="s">
         <v>9</v>
-      </c>
-      <c r="C2" s="5" t="s">
-        <v>5</v>
       </c>
       <c r="D2" s="5" t="s">
         <v>1</v>
@@ -687,13 +687,13 @@
         <v>2</v>
       </c>
       <c r="G2" s="5" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="H2" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="I2" s="5" t="s">
         <v>6</v>
-      </c>
-      <c r="I2" s="5" t="s">
-        <v>7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>